<commit_message>
completed upload and download
</commit_message>
<xml_diff>
--- a/format_question.xlsx
+++ b/format_question.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
+  <si>
+    <t>chapter_id</t>
+  </si>
   <si>
     <t>question</t>
   </si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t>time_duration</t>
+  </si>
+  <si>
+    <t>f1a3a82b-41d3-4d63-bf0d-a30a85538249</t>
   </si>
 </sst>
 </file>
@@ -372,13 +378,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="6" width="37.7109375" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" customWidth="1"/>
+    <col min="8" max="8" width="47.7109375" customWidth="1"/>
+    <col min="9" max="9" width="35.7109375" customWidth="1"/>
+    <col min="10" max="10" width="43.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,6 +420,154 @@
       </c>
       <c r="I1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>